<commit_message>
Fix forms to use CSV file instead of hard coded values for villages, subvillages, and veos, commit test data, remove unnecessary files
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="465" windowWidth="24300" windowHeight="16500" activeTab="5"/>
+    <workbookView xWindow="4215" yWindow="465" windowWidth="24300" windowHeight="16500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="172">
   <si>
     <t>comments</t>
   </si>
@@ -548,6 +548,15 @@
   </si>
   <si>
     <t>Delete</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('business','business')</t>
+  </si>
+  <si>
+    <t>Business</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1151,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1303,10 +1312,34 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
     </row>
   </sheetData>
@@ -1452,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1507,6 +1540,17 @@
       </c>
       <c r="C4" s="3" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2040,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update framework, remove unnecessary csv file, clean up
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="2760" windowWidth="24300" windowHeight="16500" activeTab="1"/>
+    <workbookView xWindow="11500" yWindow="2760" windowWidth="24300" windowHeight="16500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="169">
   <si>
     <t>comments</t>
   </si>
@@ -503,28 +503,10 @@
     <t>business_enrollment</t>
   </si>
   <si>
-    <t>business_verification</t>
-  </si>
-  <si>
-    <t>business_authorization</t>
-  </si>
-  <si>
     <t>Enrollment</t>
   </si>
   <si>
-    <t>Verification</t>
-  </si>
-  <si>
-    <t>Authorization</t>
-  </si>
-  <si>
     <t>'?' +  odkSurvey.getHashString('business','enrollment')</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('business','verification')</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('business','authorization')</t>
   </si>
   <si>
     <t>are_you_sure_you_want_to_delete_row</t>
@@ -1160,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1260,7 +1242,7 @@
     <row r="9" spans="1:9" ht="66" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>
@@ -1278,13 +1260,13 @@
     </row>
     <row r="11" spans="1:9" ht="17.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="66" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -1302,13 +1284,13 @@
     </row>
     <row r="14" spans="1:9" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="66" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -1324,59 +1306,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="66" customHeight="1">
+    <row r="17" spans="1:1" ht="12.75" customHeight="1">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" ht="12.75" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1553,7 +1487,7 @@
         <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1561,10 +1495,10 @@
         <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1572,32 +1506,10 @@
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2099,26 +2011,26 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2156,26 +2068,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a few more changes and started to add translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eKichabi\app-designer\app\config\assets\framework\forms\framework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="2760" windowWidth="24300" windowHeight="16500" activeTab="3"/>
+    <workbookView xWindow="11503" yWindow="2760" windowWidth="24300" windowHeight="16500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -15,16 +20,11 @@
     <sheet name="common_translations" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="177">
   <si>
     <t>comments</t>
   </si>
@@ -544,12 +544,36 @@
   <si>
     <t>'?' +  odkSurvey.getHashString('geo_unit','geo_unit')</t>
   </si>
+  <si>
+    <t>text.sw</t>
+  </si>
+  <si>
+    <t>Kamilisha</t>
+  </si>
+  <si>
+    <t>Isiyo kamilika</t>
+  </si>
+  <si>
+    <t>Nyuma</t>
+  </si>
+  <si>
+    <t>Mbele/Endelea</t>
+  </si>
+  <si>
+    <t>Tengeneza ukurasa mpya wa mahojiano</t>
+  </si>
+  <si>
+    <t>Nenda ukurasa unaofuata</t>
+  </si>
+  <si>
+    <t>Batilisha</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -575,6 +599,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -593,7 +624,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -689,8 +720,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -707,8 +739,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="95" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="96">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -804,6 +853,7 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="95"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1111,13 +1161,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.84375" customWidth="1"/>
+    <col min="2" max="2" width="20.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1148,19 +1198,19 @@
       <selection activeCell="A11" sqref="A11:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.15234375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="101.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.15234375" customWidth="1"/>
+    <col min="2" max="2" width="101.15234375" customWidth="1"/>
+    <col min="3" max="3" width="22.15234375" customWidth="1"/>
+    <col min="4" max="4" width="46.15234375" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21.84375" customWidth="1"/>
+    <col min="8" max="8" width="31.4609375" customWidth="1"/>
+    <col min="9" max="9" width="22.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1187,7 +1237,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -1196,7 +1246,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>21</v>
       </c>
@@ -1207,13 +1257,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -1224,22 +1274,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.5" customHeight="1">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="66" customHeight="1">
+    <row r="9" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>156</v>
@@ -1251,19 +1301,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="66" customHeight="1">
+    <row r="12" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>164</v>
@@ -1275,19 +1325,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.5" customHeight="1">
+    <row r="14" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>168</v>
@@ -1299,17 +1349,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="12.75" customHeight="1">
+    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1">
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
     </row>
   </sheetData>
@@ -1331,13 +1381,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.15234375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.69140625" customWidth="1"/>
+    <col min="4" max="4" width="41.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1404,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1363,7 +1413,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1375,7 +1425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1386,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" customHeight="1">
+    <row r="5" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1400,47 +1450,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1">
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1">
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1">
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1">
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1">
+    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
   </sheetData>
@@ -1457,18 +1507,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.4609375" customWidth="1"/>
+    <col min="2" max="2" width="22.15234375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -1479,7 +1529,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1540,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1551,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1525,522 +1575,703 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" customWidth="1"/>
-    <col min="2" max="2" width="73.1640625" customWidth="1"/>
+    <col min="1" max="1" width="49.69140625" customWidth="1"/>
+    <col min="2" max="3" width="73.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" customHeight="1">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="13" customHeight="1">
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="13" customHeight="1">
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="13" customHeight="1">
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="13" customHeight="1">
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="13" customHeight="1">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>85</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>87</v>
       </c>
       <c r="B10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="13.75" customHeight="1">
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="13.75" customHeight="1">
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>66</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>73</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>83</v>
       </c>
       <c r="B26" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.25" customHeight="1">
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>93</v>
       </c>
       <c r="B29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C31" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>98</v>
       </c>
       <c r="B33" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>99</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="156">
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="161.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>105</v>
       </c>
       <c r="B36" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>111</v>
       </c>
       <c r="B38" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>110</v>
       </c>
       <c r="B39" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>113</v>
       </c>
       <c r="B40" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>115</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>117</v>
       </c>
       <c r="B42" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
       <c r="B43" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>121</v>
       </c>
       <c r="B44" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>123</v>
       </c>
       <c r="B45" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>125</v>
       </c>
       <c r="B46" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>126</v>
       </c>
       <c r="B47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>128</v>
       </c>
       <c r="B48" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="13" customHeight="1">
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>132</v>
       </c>
       <c r="B50" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>136</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>137</v>
       </c>
       <c r="B52" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>138</v>
       </c>
       <c r="B53" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>139</v>
       </c>
       <c r="B54" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>140</v>
       </c>
       <c r="B55" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>143</v>
       </c>
       <c r="B56" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>150</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A59" s="5" t="s">
         <v>151</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>152</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>157</v>
       </c>
       <c r="B61" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>159</v>
       </c>
       <c r="B62" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63" t="s">
         <v>162</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2052,13 +2283,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2066,7 +2297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -2074,7 +2305,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -2082,7 +2313,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>

</xml_diff>

<commit_message>
Choose only one word for the next button
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -704,9 +704,6 @@
     <t>Nyuma</t>
   </si>
   <si>
-    <t>Mbele/Endelea</t>
-  </si>
-  <si>
     <t>Sina uhakika</t>
   </si>
   <si>
@@ -741,6 +738,9 @@
   </si>
   <si>
     <t>Enter the network for the phone number.</t>
+  </si>
+  <si>
+    <t>Mbele</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1865,7 +1865,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1">
@@ -2254,7 +2254,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="5" customFormat="1">
@@ -2593,7 +2593,7 @@
         <v>175</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1">
@@ -2801,46 +2801,46 @@
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1">
       <c r="A31" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>226</v>
       </c>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1">
       <c r="A32" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>227</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>228</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1">
       <c r="A33" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" s="5" customFormat="1">
       <c r="A34" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>231</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>232</v>
       </c>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1">
       <c r="A35" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>233</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>234</v>
       </c>
       <c r="C35" s="7"/>
     </row>

</xml_diff>

<commit_message>
Updated crops list and changed question to year business started instead of business age
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1640" windowWidth="29100" windowHeight="17480" activeTab="4"/>
+    <workbookView xWindow="4820" yWindow="1640" windowWidth="29100" windowHeight="17480" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -632,9 +632,6 @@
     <t>Business Owner Age</t>
   </si>
   <si>
-    <t>Business Age</t>
-  </si>
-  <si>
     <t>Firm Size</t>
   </si>
   <si>
@@ -644,9 +641,6 @@
     <t>business_owner_age</t>
   </si>
   <si>
-    <t>business_age</t>
-  </si>
-  <si>
     <t>firm_size</t>
   </si>
   <si>
@@ -741,6 +735,12 @@
   </si>
   <si>
     <t>Mbele</t>
+  </si>
+  <si>
+    <t>year_business_started</t>
+  </si>
+  <si>
+    <t>Year Business Started</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1854,7 +1854,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1">
@@ -1865,7 +1865,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1">
@@ -2115,7 +2115,7 @@
         <v>108</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="5" customFormat="1">
@@ -2207,7 +2207,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="5" customFormat="1">
@@ -2254,7 +2254,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="5" customFormat="1">
@@ -2274,7 +2274,7 @@
         <v>127</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2518,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2593,7 +2593,7 @@
         <v>175</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1">
@@ -2697,7 +2697,7 @@
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1">
       <c r="A19" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>197</v>
@@ -2706,91 +2706,91 @@
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1">
       <c r="A20" s="7" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1">
       <c r="A21" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1">
       <c r="A22" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" s="5" customFormat="1">
       <c r="A23" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1">
       <c r="A24" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1">
       <c r="A25" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" s="5" customFormat="1">
       <c r="A26" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" s="5" customFormat="1">
       <c r="A27" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1">
       <c r="A29" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C29" s="7"/>
     </row>
@@ -2801,46 +2801,46 @@
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1">
       <c r="A31" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1">
       <c r="A32" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1">
       <c r="A33" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" s="5" customFormat="1">
       <c r="A34" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C35" s="7"/>
     </row>

</xml_diff>

<commit_message>
Add in latest translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1640" windowWidth="29100" windowHeight="17480" activeTab="5"/>
+    <workbookView xWindow="5560" yWindow="11960" windowWidth="27240" windowHeight="17100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="295">
   <si>
     <t>comments</t>
   </si>
@@ -741,6 +741,198 @@
   </si>
   <si>
     <t>Year Business Started</t>
+  </si>
+  <si>
+    <t>Udhibitisho</t>
+  </si>
+  <si>
+    <t>Endelea</t>
+  </si>
+  <si>
+    <t>Chagua</t>
+  </si>
+  <si>
+    <t>Tafadhali subiri....</t>
+  </si>
+  <si>
+    <t>HAPANA</t>
+  </si>
+  <si>
+    <t>NDIYO</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mwisho wa usahili mpya: &lt;/p&gt;&lt;p&gt;"{{display_field}}"&lt;/p&gt;&lt;hr&gt;</t>
+  </si>
+  <si>
+    <t>Kamilisha</t>
+  </si>
+  <si>
+    <t>Lugha</t>
+  </si>
+  <si>
+    <t>Maudhui</t>
+  </si>
+  <si>
+    <t>Sawa</t>
+  </si>
+  <si>
+    <t>Eleza</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Iliyofanyika hapo mwanzo:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Angalia</t>
+  </si>
+  <si>
+    <t>Thamani ya namba inayotarajiwa</t>
+  </si>
+  <si>
+    <t>ukubwa wa thamani inayotarajiwa</t>
+  </si>
+  <si>
+    <t>kutoka</t>
+  </si>
+  <si>
+    <t>Batilisha</t>
+  </si>
+  <si>
+    <t>Je unauhakika unataka kutoka na kufuta  mabadiliko yote uliyofanya?</t>
+  </si>
+  <si>
+    <t>Una uhakika unataka kufuta mstari huu</t>
+  </si>
+  <si>
+    <t>Hariri</t>
+  </si>
+  <si>
+    <t>Futa</t>
+  </si>
+  <si>
+    <t>Halali</t>
+  </si>
+  <si>
+    <t>Sio halali</t>
+  </si>
+  <si>
+    <t>Uhakiki wa Mtendaji (VEO)</t>
+  </si>
+  <si>
+    <t>Wasilisha</t>
+  </si>
+  <si>
+    <t>Bado Kudhibitishwa</t>
+  </si>
+  <si>
+    <t>Zote</t>
+  </si>
+  <si>
+    <t>Tafuta</t>
+  </si>
+  <si>
+    <t>Ya nyuma</t>
+  </si>
+  <si>
+    <t>Onesha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jina </t>
+  </si>
+  <si>
+    <t>Aina ya Sekta</t>
+  </si>
+  <si>
+    <t>Jinsia</t>
+  </si>
+  <si>
+    <t>Umri wa mmiliki wa biashara</t>
+  </si>
+  <si>
+    <t>Biashara hii ilianza mwaka gani?</t>
+  </si>
+  <si>
+    <t>Biashara hii ina ukubwa gani (idadi ya waajiriwa, pasipo kujumuisha mmiliki wa biashara)?</t>
+  </si>
+  <si>
+    <t>Namba ya simu</t>
+  </si>
+  <si>
+    <t>Namba ya pili ya simu</t>
+  </si>
+  <si>
+    <t>Imehakikiwa na wakala?</t>
+  </si>
+  <si>
+    <t>Imehakikiwa na mtendaji(VEO)?</t>
+  </si>
+  <si>
+    <t>Wakala</t>
+  </si>
+  <si>
+    <t>Mtendaji</t>
+  </si>
+  <si>
+    <t>Msimimizi</t>
+  </si>
+  <si>
+    <t>Angalia Biashara</t>
+  </si>
+  <si>
+    <t>Unakubali kushiriki?</t>
+  </si>
+  <si>
+    <t>Chagua sehemu ya sekta ya biashara</t>
+  </si>
+  <si>
+    <t>Unajikita katika zao  moja au mifugo?</t>
+  </si>
+  <si>
+    <t>Jina la mmiliki wa biashara?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tathimini ya vikwazo isiyo halali(). See console log. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tathimini isiyohitajika(). See console log. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     {{#if display_field}}
+        &lt;p&gt;Mwanzo wa usahili mpya: &lt;/p&gt;
+        &lt;p&gt;"{{display_field}}"&lt;/p&gt; 
+  {{else}}
+        &lt;p&gt;Mwanzo wa usahili mpya.&lt;/p&gt;
+  {{/if}}
+        &lt;hr&gt;
+        {{#if last_save_date}}
+            &lt;p&gt;Last saved:&lt;/p&gt; 
+            &lt;p&gt;{{last_save_date}}&lt;/p&gt;
+        {{/if}}
+        &lt;hr&gt;
+</t>
+  </si>
+  <si>
+    <t>Usiruhusu mabadiliko + kutoka</t>
+  </si>
+  <si>
+    <t>Hifadhi mabadiliko + kutoka</t>
+  </si>
+  <si>
+    <t>Mwisho + kutoka</t>
+  </si>
+  <si>
+    <t>Thamani isiyo halali.</t>
+  </si>
+  <si>
+    <t>Thamani halali haijatolewa.</t>
+  </si>
+  <si>
+    <t>Hakuna dodoso lililohifadhiwa.</t>
+  </si>
+  <si>
+    <t>Andika kampuni ya mtandao wa namba ya simu.</t>
+  </si>
+  <si>
+    <t>Vikwazo vimekiukwa.</t>
   </si>
 </sst>
 </file>
@@ -812,8 +1004,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -934,9 +1132,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -946,10 +1141,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -998,6 +1196,9 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1046,6 +1247,9 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1388,7 +1592,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1768,10 +1972,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1779,6 +1983,7 @@
     <col min="1" max="1" width="49.6640625" customWidth="1"/>
     <col min="2" max="2" width="73.1640625" customWidth="1"/>
     <col min="3" max="3" width="57.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" customHeight="1">
@@ -1792,108 +1997,126 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="C2" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" s="5" customFormat="1">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="9" customFormat="1">
+      <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" s="10" customFormat="1">
-      <c r="A8" s="9" t="s">
+      <c r="C7" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="9" customFormat="1">
+      <c r="A8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="10" customFormat="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" s="9" customFormat="1">
+      <c r="A9" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="5" customFormat="1">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:3" s="9" customFormat="1">
+      <c r="A10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="9" customFormat="1" ht="13.75" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" ht="13.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="C11" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="9" customFormat="1" ht="13.75" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="6" t="s">
@@ -1940,14 +2163,16 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" s="5" customFormat="1">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:3" s="9" customFormat="1">
+      <c r="A18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="6" t="s">
@@ -2003,23 +2228,27 @@
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" s="5" customFormat="1">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:3" s="9" customFormat="1">
+      <c r="A25" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" s="5" customFormat="1">
-      <c r="A26" s="7" t="s">
+      <c r="C25" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="9" customFormat="1">
+      <c r="A26" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="8" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
@@ -2039,39 +2268,45 @@
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" s="5" customFormat="1">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:3" s="9" customFormat="1">
+      <c r="A29" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" s="5" customFormat="1">
-      <c r="A30" s="7" t="s">
+      <c r="C29" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="9" customFormat="1">
+      <c r="A30" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" s="5" customFormat="1">
-      <c r="A31" s="7" t="s">
+      <c r="C30" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="9" customFormat="1">
+      <c r="A31" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="6" t="s">
         <v>98</v>
       </c>
@@ -2080,7 +2315,7 @@
       </c>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="6" t="s">
         <v>99</v>
       </c>
@@ -2089,7 +2324,7 @@
       </c>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" s="6" t="s">
         <v>102</v>
       </c>
@@ -2098,99 +2333,118 @@
       </c>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" s="5" customFormat="1" ht="156">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="156">
       <c r="A36" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="7"/>
-    </row>
-    <row r="37" spans="1:3" s="10" customFormat="1">
-      <c r="A37" s="9" t="s">
+      <c r="C36" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" s="9" customFormat="1">
+      <c r="A37" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="5" customFormat="1">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:4" s="9" customFormat="1">
+      <c r="A38" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" s="5" customFormat="1">
-      <c r="A39" s="7" t="s">
+      <c r="C38" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="9" customFormat="1">
+      <c r="A39" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:3" s="5" customFormat="1">
-      <c r="A40" s="7" t="s">
+      <c r="C39" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="9" customFormat="1">
+      <c r="A40" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" s="5" customFormat="1">
-      <c r="A41" s="7" t="s">
+      <c r="C40" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1">
+      <c r="A41" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:3" s="5" customFormat="1">
-      <c r="A42" s="7" t="s">
+      <c r="C41" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="9" customFormat="1">
+      <c r="A42" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" s="5" customFormat="1">
-      <c r="A43" s="7" t="s">
+      <c r="C42" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1">
+      <c r="A43" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:3" s="5" customFormat="1">
-      <c r="A44" s="7" t="s">
+      <c r="C43" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="9" customFormat="1">
+      <c r="A44" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" s="5" customFormat="1">
-      <c r="A45" s="7" t="s">
+      <c r="C44" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="9" customFormat="1">
+      <c r="A45" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="C45" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="6" t="s">
         <v>125</v>
       </c>
@@ -2199,25 +2453,27 @@
       </c>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" s="10" customFormat="1">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:4" s="9" customFormat="1">
+      <c r="A47" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="5" customFormat="1">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:4" s="9" customFormat="1">
+      <c r="A48" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
       <c r="A49" s="7" t="s">
@@ -2228,14 +2484,16 @@
       </c>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="13" customHeight="1">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="A50" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="8" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="51" spans="1:3" s="5" customFormat="1">
       <c r="A51" s="7" t="s">
@@ -2246,34 +2504,36 @@
       </c>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:3" s="10" customFormat="1">
-      <c r="A52" s="9" t="s">
+    <row r="52" spans="1:3" s="9" customFormat="1">
+      <c r="A52" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="5" customFormat="1">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:3" s="9" customFormat="1">
+      <c r="A53" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" s="10" customFormat="1">
-      <c r="A54" s="9" t="s">
+      <c r="C53" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="9" customFormat="1">
+      <c r="A54" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2286,77 +2546,93 @@
       </c>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1">
-      <c r="A56" s="7" t="s">
+    <row r="56" spans="1:3" s="9" customFormat="1">
+      <c r="A56" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="1:3" s="5" customFormat="1">
-      <c r="A57" s="7" t="s">
+      <c r="C56" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="9" customFormat="1">
+      <c r="A57" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="1:3" s="5" customFormat="1">
-      <c r="A58" s="8" t="s">
+      <c r="C57" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="9" customFormat="1">
+      <c r="A58" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="1:3" s="5" customFormat="1">
-      <c r="A59" s="8" t="s">
+      <c r="C58" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="9" customFormat="1">
+      <c r="A59" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:3" s="5" customFormat="1">
-      <c r="A60" s="8" t="s">
+      <c r="C59" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="9" customFormat="1">
+      <c r="A60" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C60" s="7"/>
-    </row>
-    <row r="61" spans="1:3" s="5" customFormat="1">
-      <c r="A61" s="7" t="s">
+      <c r="C60" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="9" customFormat="1">
+      <c r="A61" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="7"/>
-    </row>
-    <row r="62" spans="1:3" s="5" customFormat="1">
-      <c r="A62" s="7" t="s">
+      <c r="C61" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="9" customFormat="1">
+      <c r="A62" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C62" s="7"/>
-    </row>
-    <row r="63" spans="1:3" s="5" customFormat="1">
-      <c r="A63" s="7" t="s">
+      <c r="C62" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="9" customFormat="1">
+      <c r="A63" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C63" s="7"/>
+      <c r="C63" s="8" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="6"/>
@@ -2518,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2540,50 +2816,60 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="9" customFormat="1">
+      <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" s="5" customFormat="1">
-      <c r="A3" s="7" t="s">
+      <c r="C2" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1">
+      <c r="A3" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" s="5" customFormat="1">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="9" customFormat="1">
+      <c r="A4" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" s="5" customFormat="1">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="9" customFormat="1">
+      <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" s="5" customFormat="1">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="9" customFormat="1">
+      <c r="A6" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
@@ -2596,253 +2882,307 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="5" customFormat="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3" s="9" customFormat="1">
+      <c r="A8" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" s="5" customFormat="1">
-      <c r="A9" s="7" t="s">
+      <c r="C8" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="9" customFormat="1">
+      <c r="A9" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" s="5" customFormat="1">
-      <c r="A10" s="7" t="s">
+      <c r="C9" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="9" customFormat="1">
+      <c r="A10" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1">
-      <c r="A11" s="7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="9" customFormat="1">
+      <c r="A11" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1">
-      <c r="A12" s="7" t="s">
+      <c r="C11" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="9" customFormat="1">
+      <c r="A12" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" s="5" customFormat="1">
-      <c r="A13" s="7" t="s">
+      <c r="C12" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="9" customFormat="1">
+      <c r="A13" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" s="5" customFormat="1">
-      <c r="A14" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="9" customFormat="1">
+      <c r="A14" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" s="5" customFormat="1">
-      <c r="A15" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="9" customFormat="1">
+      <c r="A15" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" s="5" customFormat="1">
-      <c r="A16" s="7" t="s">
+      <c r="C15" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="9" customFormat="1">
+      <c r="A16" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" s="5" customFormat="1">
-      <c r="A17" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="9" customFormat="1">
+      <c r="A17" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" s="5" customFormat="1">
-      <c r="A18" s="7" t="s">
+      <c r="C17" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="9" customFormat="1">
+      <c r="A18" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" s="5" customFormat="1">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="9" customFormat="1">
+      <c r="A19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" s="5" customFormat="1">
-      <c r="A20" s="7" t="s">
+      <c r="C19" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="9" customFormat="1">
+      <c r="A20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" s="5" customFormat="1">
-      <c r="A21" s="7" t="s">
+      <c r="C20" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="9" customFormat="1" ht="24">
+      <c r="A21" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" s="5" customFormat="1">
-      <c r="A22" s="7" t="s">
+      <c r="C21" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="9" customFormat="1">
+      <c r="A22" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" s="5" customFormat="1">
-      <c r="A23" s="7" t="s">
+      <c r="C22" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="9" customFormat="1">
+      <c r="A23" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" s="5" customFormat="1">
-      <c r="A24" s="7" t="s">
+      <c r="C23" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="9" customFormat="1">
+      <c r="A24" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:3" s="5" customFormat="1">
-      <c r="A25" s="7" t="s">
+      <c r="C24" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="9" customFormat="1">
+      <c r="A25" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" s="5" customFormat="1">
-      <c r="A26" s="7" t="s">
+      <c r="C25" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="9" customFormat="1">
+      <c r="A26" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="1:3" s="5" customFormat="1">
-      <c r="A27" s="7" t="s">
+      <c r="C26" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="9" customFormat="1">
+      <c r="A27" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" s="5" customFormat="1">
-      <c r="A28" s="7" t="s">
+      <c r="C27" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="9" customFormat="1">
+      <c r="A28" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" s="5" customFormat="1">
-      <c r="A29" s="7" t="s">
+      <c r="C28" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="9" customFormat="1">
+      <c r="A29" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" s="10" customFormat="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" s="5" customFormat="1">
-      <c r="A31" s="7" t="s">
+      <c r="C29" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="9" customFormat="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" s="9" customFormat="1">
+      <c r="A31" s="8" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" s="5" customFormat="1">
-      <c r="A32" s="7" t="s">
+      <c r="C31" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="9" customFormat="1">
+      <c r="A32" s="8" t="s">
         <v>224</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:3" s="5" customFormat="1">
-      <c r="A33" s="7" t="s">
+      <c r="C32" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="9" customFormat="1">
+      <c r="A33" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" s="5" customFormat="1">
-      <c r="A34" s="7" t="s">
+      <c r="C33" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="9" customFormat="1">
+      <c r="A34" s="8" t="s">
         <v>228</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" s="5" customFormat="1">
-      <c r="A35" s="7" t="s">
+      <c r="C34" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="9" customFormat="1">
+      <c r="A35" s="8" t="s">
         <v>230</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="8" t="s">
+        <v>293</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update app with all translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="11960" windowWidth="27240" windowHeight="17100" activeTab="4"/>
+    <workbookView xWindow="23580" yWindow="6400" windowWidth="27240" windowHeight="17100" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
     <sheet name="common_translations" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="349">
   <si>
     <t>comments</t>
   </si>
@@ -934,12 +934,174 @@
   <si>
     <t>Vikwazo vimekiukwa.</t>
   </si>
+  <si>
+    <t>agent_options</t>
+  </si>
+  <si>
+    <t>Agent Options</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>sw:Agent Options</t>
+  </si>
+  <si>
+    <t>sw:Registration</t>
+  </si>
+  <si>
+    <t>registration</t>
+  </si>
+  <si>
+    <t>pending_authorization</t>
+  </si>
+  <si>
+    <t>Pending Authorization</t>
+  </si>
+  <si>
+    <t>sw:Pending Authorization</t>
+  </si>
+  <si>
+    <t>coordinator_options</t>
+  </si>
+  <si>
+    <t>Coordinator Options</t>
+  </si>
+  <si>
+    <t>sw:Coordinator Options</t>
+  </si>
+  <si>
+    <t>welcome_to_ekichabi</t>
+  </si>
+  <si>
+    <t>Welcome to eKichabi</t>
+  </si>
+  <si>
+    <t>sw:Welcome to eKichabi</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kijiji</t>
+  </si>
+  <si>
+    <t>sign_up_for_ekichabi</t>
+  </si>
+  <si>
+    <t>Sign Up For eKichabi</t>
+  </si>
+  <si>
+    <t>sw:Sign Up For eKichabi</t>
+  </si>
+  <si>
+    <t>Biashara</t>
+  </si>
+  <si>
+    <t>coordinator_verification</t>
+  </si>
+  <si>
+    <t>Coordinator Verification</t>
+  </si>
+  <si>
+    <t>sw:Coordinator Verification</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Mkoa</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Wilaya</t>
+  </si>
+  <si>
+    <t>ward</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Kata</t>
+  </si>
+  <si>
+    <t>verified_by_coordinator</t>
+  </si>
+  <si>
+    <t>Verified by Coordinator?</t>
+  </si>
+  <si>
+    <t>sw:Verified by Coordinator?</t>
+  </si>
+  <si>
+    <t>display.title.text.english</t>
+  </si>
+  <si>
+    <t>display.title.text.sw</t>
+  </si>
+  <si>
+    <t>sw:Common Javascript Framework</t>
+  </si>
+  <si>
+    <t>display.locale.text.english</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>display.locale.text.sw</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>Swahili</t>
+  </si>
+  <si>
+    <t>Kiingereza</t>
+  </si>
+  <si>
+    <t>Kiswahili</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>valid_business</t>
+  </si>
+  <si>
+    <t>Valid Business</t>
+  </si>
+  <si>
+    <t>sw:Valid Business</t>
+  </si>
+  <si>
+    <t>invalid_business</t>
+  </si>
+  <si>
+    <t>Invalid Business</t>
+  </si>
+  <si>
+    <t>sw:Invalid Business</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -964,6 +1126,25 @@
       <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1004,7 +1185,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1108,8 +1289,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1146,8 +1343,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1199,6 +1406,14 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1250,6 +1465,14 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1772,19 +1995,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" customWidth="1"/>
+    <col min="3" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="6" width="24.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1792,16 +2016,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1809,8 +2042,11 @@
         <v>31</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1818,22 +2054,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>20180703</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" customHeight="1">
+    <row r="5" spans="1:8" ht="28" customHeight="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1841,57 +2080,86 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>334</v>
+      </c>
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="b">
+      <c r="H5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="12.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="12.75" customHeight="1">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1">
       <c r="A14" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:4" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1">
+    <row r="20" spans="1:4" ht="12.75" customHeight="1">
       <c r="A20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1905,7 +2173,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1974,7 +2242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2792,10 +3060,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3184,8 +3452,174 @@
         <v>293</v>
       </c>
     </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>295</v>
+      </c>
+      <c r="B37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>300</v>
+      </c>
+      <c r="B38" t="s">
+        <v>297</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>301</v>
+      </c>
+      <c r="B39" t="s">
+        <v>302</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>304</v>
+      </c>
+      <c r="B41" t="s">
+        <v>305</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" t="s">
+        <v>308</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>310</v>
+      </c>
+      <c r="B44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C44" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13">
+      <c r="A45" t="s">
+        <v>313</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>317</v>
+      </c>
+      <c r="B48" t="s">
+        <v>318</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>320</v>
+      </c>
+      <c r="B50" t="s">
+        <v>321</v>
+      </c>
+      <c r="C50" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>323</v>
+      </c>
+      <c r="B51" t="s">
+        <v>324</v>
+      </c>
+      <c r="C51" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>326</v>
+      </c>
+      <c r="B52" t="s">
+        <v>327</v>
+      </c>
+      <c r="C52" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="13">
+      <c r="A54" t="s">
+        <v>329</v>
+      </c>
+      <c r="B54" t="s">
+        <v>330</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>343</v>
+      </c>
+      <c r="B56" t="s">
+        <v>344</v>
+      </c>
+      <c r="C56" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>346</v>
+      </c>
+      <c r="B57" t="s">
+        <v>347</v>
+      </c>
+      <c r="C57" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add business owner name to detail view
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -14,7 +14,7 @@
     <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
     <sheet name="common_translations" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -725,9 +725,6 @@
     <t>business_owner_name</t>
   </si>
   <si>
-    <t xml:space="preserve">What is the business owners name? </t>
-  </si>
-  <si>
     <t>network_phone</t>
   </si>
   <si>
@@ -885,9 +882,6 @@
   </si>
   <si>
     <t>Unajikita katika zao  moja au mifugo?</t>
-  </si>
-  <si>
-    <t>Jina la mmiliki wa biashara?</t>
   </si>
   <si>
     <t xml:space="preserve">Tathimini ya vikwazo isiyo halali(). See console log. </t>
@@ -1095,6 +1089,12 @@
   </si>
   <si>
     <t>sw:Invalid Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business owner name </t>
+  </si>
+  <si>
+    <t>Jina la mmiliki wa biashara</t>
   </si>
 </sst>
 </file>
@@ -1814,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2016,16 +2016,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>337</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -2080,7 +2080,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -2097,24 +2097,24 @@
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>338</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>339</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1">
@@ -2242,7 +2242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2273,7 +2273,7 @@
         <v>47</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
@@ -2284,7 +2284,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
@@ -2295,7 +2295,7 @@
         <v>49</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
@@ -2306,7 +2306,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="9" customFormat="1" ht="13" customHeight="1">
@@ -2317,7 +2317,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1">
@@ -2328,7 +2328,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="9" customFormat="1">
@@ -2350,7 +2350,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="9" customFormat="1">
@@ -2361,7 +2361,7 @@
         <v>88</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="9" customFormat="1" ht="13.75" customHeight="1">
@@ -2372,7 +2372,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="9" customFormat="1" ht="13.75" customHeight="1">
@@ -2383,7 +2383,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2439,7 +2439,7 @@
         <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2504,7 +2504,7 @@
         <v>82</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="9" customFormat="1">
@@ -2515,7 +2515,7 @@
         <v>84</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2544,7 +2544,7 @@
         <v>91</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="9" customFormat="1">
@@ -2555,7 +2555,7 @@
         <v>95</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="9" customFormat="1">
@@ -2609,7 +2609,7 @@
         <v>106</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D36" s="7"/>
     </row>
@@ -2632,7 +2632,7 @@
         <v>109</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="9" customFormat="1">
@@ -2643,7 +2643,7 @@
         <v>112</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="9" customFormat="1">
@@ -2654,7 +2654,7 @@
         <v>114</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="9" customFormat="1">
@@ -2665,7 +2665,7 @@
         <v>116</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="9" customFormat="1">
@@ -2676,7 +2676,7 @@
         <v>118</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="9" customFormat="1">
@@ -2687,7 +2687,7 @@
         <v>120</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="9" customFormat="1">
@@ -2698,7 +2698,7 @@
         <v>122</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="9" customFormat="1">
@@ -2709,7 +2709,7 @@
         <v>38</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2740,7 +2740,7 @@
         <v>129</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
@@ -2760,7 +2760,7 @@
         <v>133</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="5" customFormat="1">
@@ -2791,7 +2791,7 @@
         <v>135</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="9" customFormat="1">
@@ -2822,7 +2822,7 @@
         <v>144</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1">
@@ -2833,7 +2833,7 @@
         <v>145</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="9" customFormat="1">
@@ -2844,7 +2844,7 @@
         <v>148</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="9" customFormat="1">
@@ -2855,7 +2855,7 @@
         <v>149</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="9" customFormat="1">
@@ -2866,7 +2866,7 @@
         <v>153</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1">
@@ -2877,7 +2877,7 @@
         <v>158</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="9" customFormat="1">
@@ -2888,7 +2888,7 @@
         <v>160</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="9" customFormat="1">
@@ -2899,7 +2899,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -3062,8 +3062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3092,7 +3092,7 @@
         <v>158</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="9" customFormat="1">
@@ -3103,7 +3103,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1">
@@ -3114,7 +3114,7 @@
         <v>162</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="9" customFormat="1">
@@ -3125,7 +3125,7 @@
         <v>173</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="9" customFormat="1">
@@ -3136,7 +3136,7 @@
         <v>174</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3158,7 +3158,7 @@
         <v>178</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="9" customFormat="1">
@@ -3169,7 +3169,7 @@
         <v>179</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="9" customFormat="1">
@@ -3180,7 +3180,7 @@
         <v>181</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="9" customFormat="1">
@@ -3191,7 +3191,7 @@
         <v>184</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="9" customFormat="1">
@@ -3202,7 +3202,7 @@
         <v>185</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="9" customFormat="1">
@@ -3213,7 +3213,7 @@
         <v>192</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="9" customFormat="1">
@@ -3224,7 +3224,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1">
@@ -3235,7 +3235,7 @@
         <v>191</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="9" customFormat="1">
@@ -3246,7 +3246,7 @@
         <v>190</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">
@@ -3257,7 +3257,7 @@
         <v>194</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="9" customFormat="1">
@@ -3268,7 +3268,7 @@
         <v>196</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="9" customFormat="1">
@@ -3279,18 +3279,18 @@
         <v>197</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1">
       <c r="A20" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>234</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="9" customFormat="1" ht="24">
@@ -3301,7 +3301,7 @@
         <v>198</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="9" customFormat="1">
@@ -3312,7 +3312,7 @@
         <v>199</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1">
@@ -3323,7 +3323,7 @@
         <v>206</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="9" customFormat="1">
@@ -3334,7 +3334,7 @@
         <v>207</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="9" customFormat="1">
@@ -3345,7 +3345,7 @@
         <v>208</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="9" customFormat="1">
@@ -3356,7 +3356,7 @@
         <v>210</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1">
@@ -3367,7 +3367,7 @@
         <v>212</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="9" customFormat="1">
@@ -3378,7 +3378,7 @@
         <v>214</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="9" customFormat="1">
@@ -3389,7 +3389,7 @@
         <v>216</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="9" customFormat="1">
@@ -3405,7 +3405,7 @@
         <v>223</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="9" customFormat="1">
@@ -3416,7 +3416,7 @@
         <v>225</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="9" customFormat="1">
@@ -3427,7 +3427,7 @@
         <v>227</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1">
@@ -3435,98 +3435,98 @@
         <v>228</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>229</v>
+        <v>347</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>283</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="9" customFormat="1">
       <c r="A35" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>231</v>
-      </c>
       <c r="C35" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B37" t="s">
+        <v>294</v>
+      </c>
+      <c r="C37" s="14" t="s">
         <v>296</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B38" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>297</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" t="s">
+        <v>300</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="B39" t="s">
-        <v>302</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>302</v>
+      </c>
+      <c r="B41" t="s">
+        <v>303</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="B41" t="s">
-        <v>305</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>305</v>
+      </c>
+      <c r="B42" t="s">
+        <v>306</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="B42" t="s">
-        <v>308</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>308</v>
+      </c>
+      <c r="B44" t="s">
+        <v>309</v>
+      </c>
+      <c r="C44" t="s">
         <v>310</v>
-      </c>
-      <c r="B44" t="s">
-        <v>311</v>
-      </c>
-      <c r="C44" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="13">
       <c r="A45" t="s">
+        <v>311</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>313</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -3537,84 +3537,84 @@
         <v>165</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>315</v>
+      </c>
+      <c r="B48" t="s">
+        <v>316</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>317</v>
-      </c>
-      <c r="B48" t="s">
-        <v>318</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>318</v>
+      </c>
+      <c r="B50" t="s">
+        <v>319</v>
+      </c>
+      <c r="C50" t="s">
         <v>320</v>
-      </c>
-      <c r="B50" t="s">
-        <v>321</v>
-      </c>
-      <c r="C50" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>321</v>
+      </c>
+      <c r="B51" t="s">
+        <v>322</v>
+      </c>
+      <c r="C51" t="s">
         <v>323</v>
-      </c>
-      <c r="B51" t="s">
-        <v>324</v>
-      </c>
-      <c r="C51" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>324</v>
+      </c>
+      <c r="B52" t="s">
+        <v>325</v>
+      </c>
+      <c r="C52" t="s">
         <v>326</v>
-      </c>
-      <c r="B52" t="s">
-        <v>327</v>
-      </c>
-      <c r="C52" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="13">
       <c r="A54" t="s">
+        <v>327</v>
+      </c>
+      <c r="B54" t="s">
+        <v>328</v>
+      </c>
+      <c r="C54" s="16" t="s">
         <v>329</v>
-      </c>
-      <c r="B54" t="s">
-        <v>330</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>341</v>
+      </c>
+      <c r="B56" t="s">
+        <v>342</v>
+      </c>
+      <c r="C56" t="s">
         <v>343</v>
-      </c>
-      <c r="B56" t="s">
-        <v>344</v>
-      </c>
-      <c r="C56" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>344</v>
+      </c>
+      <c r="B57" t="s">
+        <v>345</v>
+      </c>
+      <c r="C57" t="s">
         <v>346</v>
-      </c>
-      <c r="B57" t="s">
-        <v>347</v>
-      </c>
-      <c r="C57" t="s">
-        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished medical consult demo
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randy\Desktop\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaochongbin/WebstormProjects/app-designer11/app/config/assets/framework/forms/framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC0E4BD-EB3A-489C-B168-0B2EEAB61E03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8A4338-75F2-5A4D-85C3-BCE09D307F44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="307">
   <si>
     <t>comments</t>
   </si>
@@ -966,12 +966,28 @@
   <si>
     <t>अंग्रेज़ी</t>
   </si>
+  <si>
+    <t>test_forms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>medical_consult</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medical Consultation</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('medical_consult')</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1004,6 +1020,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1153,7 +1175,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1183,137 +1205,140 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="129">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="128" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1329,7 +1354,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1651,17 +1676,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1669,12 +1694,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1686,26 +1712,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="4"/>
-    <col min="2" max="2" width="101.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="4"/>
+    <col min="2" max="2" width="101.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" style="4" customWidth="1"/>
     <col min="5" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="17.109375" style="4"/>
+    <col min="7" max="7" width="21.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="17.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -1732,7 +1758,7 @@
       </c>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1741,7 +1767,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1752,13 +1778,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1">
       <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1">
       <c r="E5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1769,23 +1795,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1">
       <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1">
       <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>158</v>
@@ -1797,20 +1823,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>159</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>160</v>
@@ -1822,20 +1848,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>161</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>162</v>
@@ -1847,20 +1873,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>163</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>164</v>
@@ -1872,20 +1898,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>165</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>166</v>
@@ -1897,19 +1923,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
         <v>167</v>
@@ -1921,19 +1947,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="6" t="s">
         <v>169</v>
@@ -1945,19 +1971,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
         <v>171</v>
@@ -1969,19 +1995,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="6" t="s">
         <v>173</v>
@@ -1993,19 +2019,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>175</v>
@@ -2017,19 +2043,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="6" t="s">
         <v>177</v>
@@ -2041,19 +2067,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="6" t="s">
         <v>179</v>
@@ -2065,19 +2091,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="5"/>
       <c r="B45" s="6" t="s">
         <v>181</v>
@@ -2089,19 +2115,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
         <v>182</v>
@@ -2113,19 +2139,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="5"/>
       <c r="B51" s="6" t="s">
         <v>184</v>
@@ -2137,19 +2163,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="5"/>
       <c r="B54" s="6" t="s">
         <v>186</v>
@@ -2161,19 +2187,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="5"/>
       <c r="B57" s="6" t="s">
         <v>188</v>
@@ -2185,19 +2211,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="66" customHeight="1">
       <c r="A60" s="5"/>
       <c r="B60" s="6" t="s">
         <v>190</v>
@@ -2209,19 +2235,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="17.5" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="66" customHeight="1">
       <c r="A63" s="5"/>
       <c r="B63" s="6" t="s">
         <v>192</v>
@@ -2233,19 +2259,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="17.5" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="66" customHeight="1">
       <c r="A66" s="5"/>
       <c r="B66" s="6" t="s">
         <v>194</v>
@@ -2257,19 +2283,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="17.5" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="66" customHeight="1">
       <c r="A69" s="5"/>
       <c r="B69" s="6" t="s">
         <v>196</v>
@@ -2281,19 +2307,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="17.5" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="66" customHeight="1">
       <c r="A72" s="5"/>
       <c r="B72" s="6" t="s">
         <v>198</v>
@@ -2305,19 +2331,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="17" customHeight="1">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="12.75" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="62" customHeight="1">
       <c r="A75" s="5"/>
       <c r="B75" s="6" t="s">
         <v>200</v>
@@ -2329,19 +2355,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="12.75" customHeight="1">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="12.75" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="62" customHeight="1">
       <c r="A78" s="5"/>
       <c r="B78" s="6" t="s">
         <v>202</v>
@@ -2353,19 +2379,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="12.75" customHeight="1">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="12" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="58" customHeight="1">
       <c r="A81" s="5"/>
       <c r="B81" s="6" t="s">
         <v>204</v>
@@ -2377,19 +2403,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="12.75" customHeight="1">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="12" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="58" customHeight="1">
       <c r="A84" s="5"/>
       <c r="B84" s="6" t="s">
         <v>206</v>
@@ -2401,19 +2427,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="12.75" customHeight="1">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="12" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="58" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="6" t="s">
         <v>208</v>
@@ -2425,14 +2451,39 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="12.75" customHeight="1">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="4" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="89" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A89" s="9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="58" customHeight="1">
+      <c r="A90" s="5"/>
+      <c r="B90" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2447,17 +2498,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="3" max="8" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="41.109375" customWidth="1"/>
+    <col min="9" max="9" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2489,7 +2540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2554,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2520,7 +2571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2531,7 +2582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28" customHeight="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2551,8 +2602,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1"/>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -2566,7 +2617,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1">
       <c r="A8" t="s">
         <v>297</v>
       </c>
@@ -2580,7 +2631,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -2594,7 +2645,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2604,13 +2655,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2620,7 +2671,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2630,13 +2681,13 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2646,7 +2697,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2656,13 +2707,14 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
@@ -2675,20 +2727,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2699,7 +2751,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -2710,7 +2762,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -2721,7 +2773,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2732,7 +2784,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -2743,7 +2795,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -2765,7 +2817,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -2776,7 +2828,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2787,7 +2839,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2798,7 +2850,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2809,7 +2861,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="14">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2820,7 +2872,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2831,7 +2883,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -2842,7 +2894,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="14">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2853,7 +2905,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="14">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -2864,7 +2916,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -2875,7 +2927,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2886,7 +2938,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2897,7 +2949,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -2908,7 +2960,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -2919,7 +2971,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2930,7 +2982,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2941,7 +2993,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2952,7 +3004,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2963,7 +3015,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="14">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2974,7 +3026,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2985,7 +3037,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2996,7 +3048,19 @@
         <v>223</v>
       </c>
     </row>
+    <row r="29" spans="1:3" ht="14">
+      <c r="A29" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -3011,20 +3075,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="26.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.109375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="57.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.1640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -3038,7 +3102,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -3049,7 +3113,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -3060,7 +3124,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
@@ -3071,7 +3135,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -3082,7 +3146,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3093,7 +3157,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -3107,7 +3171,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="14">
       <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
@@ -3121,7 +3185,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14">
       <c r="A9" s="4" t="s">
         <v>86</v>
       </c>
@@ -3135,7 +3199,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -3149,7 +3213,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>124</v>
       </c>
@@ -3160,7 +3224,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -3171,7 +3235,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="14">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
@@ -3182,7 +3246,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3193,7 +3257,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
@@ -3204,7 +3268,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="14">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -3215,7 +3279,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="14">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
@@ -3226,7 +3290,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="14">
       <c r="A18" s="4" t="s">
         <v>67</v>
       </c>
@@ -3237,7 +3301,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="14">
       <c r="A19" s="4" t="s">
         <v>69</v>
       </c>
@@ -3248,7 +3312,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="14">
       <c r="A20" s="4" t="s">
         <v>71</v>
       </c>
@@ -3259,7 +3323,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="14">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -3270,7 +3334,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="14">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -3281,7 +3345,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="14">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -3292,7 +3356,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="14">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -3303,7 +3367,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="14">
       <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
@@ -3314,7 +3378,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="14">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
@@ -3325,7 +3389,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="14">
       <c r="A27" s="4" t="s">
         <v>90</v>
       </c>
@@ -3336,7 +3400,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="50.25" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>104</v>
       </c>
@@ -3347,7 +3411,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="14">
       <c r="A29" s="4" t="s">
         <v>93</v>
       </c>
@@ -3358,7 +3422,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="14">
       <c r="A30" s="4" t="s">
         <v>94</v>
       </c>
@@ -3369,7 +3433,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28">
       <c r="A31" s="4" t="s">
         <v>96</v>
       </c>
@@ -3380,7 +3444,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="14">
       <c r="A33" s="4" t="s">
         <v>98</v>
       </c>
@@ -3391,7 +3455,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="14">
       <c r="A34" s="4" t="s">
         <v>99</v>
       </c>
@@ -3402,7 +3466,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="14">
       <c r="A35" s="4" t="s">
         <v>102</v>
       </c>
@@ -3413,7 +3477,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="224">
       <c r="A36" s="4" t="s">
         <v>105</v>
       </c>
@@ -3424,7 +3488,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="28">
       <c r="A37" s="4" t="s">
         <v>107</v>
       </c>
@@ -3435,7 +3499,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="28">
       <c r="A38" s="4" t="s">
         <v>111</v>
       </c>
@@ -3446,7 +3510,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="28">
       <c r="A39" s="4" t="s">
         <v>110</v>
       </c>
@@ -3457,7 +3521,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28">
       <c r="A40" s="4" t="s">
         <v>113</v>
       </c>
@@ -3468,7 +3532,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="28">
       <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
@@ -3479,7 +3543,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="28">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
@@ -3490,7 +3554,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="14">
       <c r="A43" s="4" t="s">
         <v>119</v>
       </c>
@@ -3501,7 +3565,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="14">
       <c r="A44" s="4" t="s">
         <v>121</v>
       </c>
@@ -3512,7 +3576,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="14">
       <c r="A45" s="4" t="s">
         <v>123</v>
       </c>
@@ -3526,7 +3590,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="14">
       <c r="A46" s="4" t="s">
         <v>125</v>
       </c>
@@ -3537,7 +3601,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="28">
       <c r="A47" s="4" t="s">
         <v>126</v>
       </c>
@@ -3548,7 +3612,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="28">
       <c r="A48" s="4" t="s">
         <v>128</v>
       </c>
@@ -3559,7 +3623,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="14">
       <c r="A49" s="4" t="s">
         <v>130</v>
       </c>
@@ -3570,7 +3634,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="13" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>132</v>
       </c>
@@ -3581,7 +3645,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="28">
       <c r="A51" s="4" t="s">
         <v>136</v>
       </c>
@@ -3592,7 +3656,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="28">
       <c r="A52" s="4" t="s">
         <v>137</v>
       </c>
@@ -3603,7 +3667,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="28">
       <c r="A53" s="4" t="s">
         <v>138</v>
       </c>
@@ -3614,7 +3678,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="28">
       <c r="A54" s="4" t="s">
         <v>139</v>
       </c>
@@ -3625,7 +3689,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="14">
       <c r="A55" s="4" t="s">
         <v>140</v>
       </c>
@@ -3636,7 +3700,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="14">
       <c r="A56" s="4" t="s">
         <v>143</v>
       </c>
@@ -3647,7 +3711,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="14">
       <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
@@ -3658,7 +3722,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="14">
       <c r="A58" s="9" t="s">
         <v>150</v>
       </c>
@@ -3669,7 +3733,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="14">
       <c r="A59" s="9" t="s">
         <v>151</v>
       </c>
@@ -3680,7 +3744,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="14">
       <c r="A60" s="9" t="s">
         <v>152</v>
       </c>
@@ -3692,6 +3756,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -3710,16 +3775,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -3737,6 +3802,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added login and medical consultation
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaochongbin/WebstormProjects/app-designer11/app/config/assets/framework/forms/framework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\Research\app-designer\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8A4338-75F2-5A4D-85C3-BCE09D307F44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBBE458-7323-4AA7-A3D0-584CD998CD02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
     <sheet name="common_translations" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="310">
   <si>
     <t>comments</t>
   </si>
@@ -971,16 +971,22 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>medical_consult</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <t>registration</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('registration')</t>
+  </si>
+  <si>
+    <t>consultation</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('consultation')</t>
   </si>
   <si>
     <t>Medical Consultation</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('medical_consult')</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1210,135 +1216,135 @@
     </xf>
   </cellXfs>
   <cellStyles count="129">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1354,7 +1360,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1676,17 +1682,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1712,23 +1718,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD91"/>
+    <sheetView topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="4"/>
-    <col min="2" max="2" width="101.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" style="4"/>
+    <col min="2" max="2" width="101.1796875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" style="4" customWidth="1"/>
     <col min="5" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="31.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="17.1640625" style="4"/>
+    <col min="7" max="7" width="21.81640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="17.1796875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.5" customHeight="1">
@@ -2477,8 +2483,30 @@
     </row>
     <row r="91" spans="1:7" ht="12.75" customHeight="1">
       <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="4" t="s">
+      <c r="B91" s="11"/>
+      <c r="C91" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="12.5" customHeight="1">
+      <c r="A92" s="9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="58.5" customHeight="1">
+      <c r="A93" s="5"/>
+      <c r="B93" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C94" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2499,13 +2527,13 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="3" max="8" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="41.1640625" customWidth="1"/>
+    <col min="3" max="8" width="24.6328125" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1">
@@ -2727,20 +2755,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2751,7 +2779,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -2795,7 +2823,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2806,7 +2834,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -2817,7 +2845,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -2828,7 +2856,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2839,7 +2867,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2850,7 +2878,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2861,7 +2889,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2872,7 +2900,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2883,7 +2911,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -2894,7 +2922,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2905,7 +2933,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -2916,7 +2944,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14">
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -2927,7 +2955,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14">
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2938,7 +2966,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14">
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2949,7 +2977,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -2960,7 +2988,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14">
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -2971,7 +2999,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2982,7 +3010,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2993,7 +3021,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3004,7 +3032,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3015,7 +3043,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3026,7 +3054,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3037,7 +3065,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3048,7 +3076,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14">
+    <row r="29" spans="1:3">
       <c r="A29" s="10" t="s">
         <v>303</v>
       </c>
@@ -3057,6 +3085,17 @@
       </c>
       <c r="C29" s="10" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3075,17 +3114,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.1640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="26.36328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.81640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.1796875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" customHeight="1">
@@ -3157,7 +3196,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28">
+    <row r="7" spans="1:4" ht="25">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -3171,7 +3210,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14">
+    <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
@@ -3185,7 +3224,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14">
+    <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
         <v>86</v>
       </c>
@@ -3199,7 +3238,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14">
+    <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -3235,7 +3274,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14">
+    <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
@@ -3246,7 +3285,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14">
+    <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3257,7 +3296,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14">
+    <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
@@ -3268,7 +3307,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14">
+    <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -3279,7 +3318,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
@@ -3290,7 +3329,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14">
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
         <v>67</v>
       </c>
@@ -3301,7 +3340,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14">
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
         <v>69</v>
       </c>
@@ -3312,7 +3351,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14">
+    <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
         <v>71</v>
       </c>
@@ -3323,7 +3362,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14">
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -3334,7 +3373,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14">
+    <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -3345,7 +3384,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14">
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -3356,7 +3395,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -3367,7 +3406,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14">
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
@@ -3378,7 +3417,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14">
+    <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
@@ -3389,7 +3428,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14">
+    <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
         <v>90</v>
       </c>
@@ -3411,7 +3450,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14">
+    <row r="29" spans="1:4" ht="25">
       <c r="A29" s="4" t="s">
         <v>93</v>
       </c>
@@ -3422,7 +3461,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14">
+    <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
         <v>94</v>
       </c>
@@ -3433,7 +3472,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28">
+    <row r="31" spans="1:4" ht="25">
       <c r="A31" s="4" t="s">
         <v>96</v>
       </c>
@@ -3444,7 +3483,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14">
+    <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
         <v>98</v>
       </c>
@@ -3455,7 +3494,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14">
+    <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
         <v>99</v>
       </c>
@@ -3466,7 +3505,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14">
+    <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>102</v>
       </c>
@@ -3477,7 +3516,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="224">
+    <row r="36" spans="1:4" ht="175">
       <c r="A36" s="4" t="s">
         <v>105</v>
       </c>
@@ -3488,7 +3527,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28">
+    <row r="37" spans="1:4" ht="25">
       <c r="A37" s="4" t="s">
         <v>107</v>
       </c>
@@ -3499,7 +3538,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28">
+    <row r="38" spans="1:4" ht="25">
       <c r="A38" s="4" t="s">
         <v>111</v>
       </c>
@@ -3510,7 +3549,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28">
+    <row r="39" spans="1:4" ht="25">
       <c r="A39" s="4" t="s">
         <v>110</v>
       </c>
@@ -3521,7 +3560,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28">
+    <row r="40" spans="1:4" ht="25">
       <c r="A40" s="4" t="s">
         <v>113</v>
       </c>
@@ -3532,7 +3571,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28">
+    <row r="41" spans="1:4" ht="25">
       <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
@@ -3543,7 +3582,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="28">
+    <row r="42" spans="1:4" ht="25">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
@@ -3554,7 +3593,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14">
+    <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
         <v>119</v>
       </c>
@@ -3565,7 +3604,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14">
+    <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
         <v>121</v>
       </c>
@@ -3576,7 +3615,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14">
+    <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
         <v>123</v>
       </c>
@@ -3590,7 +3629,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="14">
+    <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
         <v>125</v>
       </c>
@@ -3601,7 +3640,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="28">
+    <row r="47" spans="1:4" ht="25">
       <c r="A47" s="4" t="s">
         <v>126</v>
       </c>
@@ -3612,7 +3651,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="28">
+    <row r="48" spans="1:4" ht="25">
       <c r="A48" s="4" t="s">
         <v>128</v>
       </c>
@@ -3623,7 +3662,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="14">
+    <row r="49" spans="1:4" ht="25">
       <c r="A49" s="4" t="s">
         <v>130</v>
       </c>
@@ -3645,7 +3684,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28">
+    <row r="51" spans="1:4" ht="25">
       <c r="A51" s="4" t="s">
         <v>136</v>
       </c>
@@ -3656,7 +3695,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28">
+    <row r="52" spans="1:4" ht="25">
       <c r="A52" s="4" t="s">
         <v>137</v>
       </c>
@@ -3667,7 +3706,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="28">
+    <row r="53" spans="1:4" ht="25">
       <c r="A53" s="4" t="s">
         <v>138</v>
       </c>
@@ -3678,7 +3717,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28">
+    <row r="54" spans="1:4" ht="25">
       <c r="A54" s="4" t="s">
         <v>139</v>
       </c>
@@ -3689,7 +3728,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="14">
+    <row r="55" spans="1:4">
       <c r="A55" s="4" t="s">
         <v>140</v>
       </c>
@@ -3700,7 +3739,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="14">
+    <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
         <v>143</v>
       </c>
@@ -3711,7 +3750,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="14">
+    <row r="57" spans="1:4">
       <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
@@ -3722,7 +3761,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="14">
+    <row r="58" spans="1:4">
       <c r="A58" s="9" t="s">
         <v>150</v>
       </c>
@@ -3733,7 +3772,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="14">
+    <row r="59" spans="1:4">
       <c r="A59" s="9" t="s">
         <v>151</v>
       </c>
@@ -3744,7 +3783,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="14">
+    <row r="60" spans="1:4">
       <c r="A60" s="9" t="s">
         <v>152</v>
       </c>
@@ -3772,19 +3811,19 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Deleted old files and created prototype
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\Research\app-designer\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBBE458-7323-4AA7-A3D0-584CD998CD02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5356F5-9D5E-4B3F-BE8D-02296174A0FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3220" yWindow="1050" windowWidth="14400" windowHeight="7810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
     <sheet name="common_translations" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="265">
   <si>
     <t>comments</t>
   </si>
@@ -509,211 +509,7 @@
     <t>English</t>
   </si>
   <si>
-    <t>exampleForm</t>
-  </si>
-  <si>
-    <t>gridScreen</t>
-  </si>
-  <si>
-    <t>agriculture</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('agriculture')</t>
-  </si>
-  <si>
-    <t>geotagger</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('geotagger')</t>
-  </si>
-  <si>
-    <t>breathcounter</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('breathcounter')</t>
-  </si>
-  <si>
-    <t>complex_validate_test</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('complex_validate_test')</t>
-  </si>
-  <si>
-    <t>customAppearance</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('customAppearance')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('exampleForm')</t>
-  </si>
-  <si>
-    <t>household</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('household')</t>
-  </si>
-  <si>
-    <t>imnci_test</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('imnci','imnci_test')</t>
-  </si>
-  <si>
-    <t>refrigerators_init</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('refrigerators','refrigerators_init')</t>
-  </si>
-  <si>
-    <t>refrigerators_update</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('refrigerators','refrigerators_update')</t>
-  </si>
-  <si>
-    <t>section_test</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('section_test')</t>
-  </si>
-  <si>
-    <t>selects</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('selects')</t>
-  </si>
-  <si>
-    <t>twoColumn</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('twoColumn')</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('gridScreen')</t>
-  </si>
-  <si>
-    <t>adult_coverage</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('adult_coverage')</t>
-  </si>
-  <si>
-    <t>child_coverage</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('child_coverage')</t>
-  </si>
-  <si>
-    <t>graphExample</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('graphExample')</t>
-  </si>
-  <si>
-    <t>visit</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('visit')</t>
-  </si>
-  <si>
-    <t>plot</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('plot')</t>
-  </si>
-  <si>
-    <t>geoweather</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('geoweather')</t>
-  </si>
-  <si>
-    <t>send_sms</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('send_sms')</t>
-  </si>
-  <si>
-    <t>eonasdan</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('eonasdan')</t>
-  </si>
-  <si>
-    <t>screenClient</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('femaleClients', 'screenClient')</t>
-  </si>
-  <si>
-    <t>client6Week</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('femaleClients','client6Week')</t>
-  </si>
-  <si>
-    <t>client6Month</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('femaleClients', 'client6Month')</t>
-  </si>
-  <si>
-    <t>screenPartner</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('maleClients', 'screenPartner')</t>
-  </si>
-  <si>
-    <t>partner6Month</t>
-  </si>
-  <si>
-    <t>'?' +  odkSurvey.getHashString('maleClients','partner6Month')</t>
-  </si>
-  <si>
     <t>Hindi</t>
-  </si>
-  <si>
-    <t>Geotagger</t>
-  </si>
-  <si>
-    <t>Child Coverage Immunizations</t>
-  </si>
-  <si>
-    <t>Adult Coverage Immunizations</t>
-  </si>
-  <si>
-    <t>Graph Examples</t>
-  </si>
-  <si>
-    <t>Visit</t>
-  </si>
-  <si>
-    <t>Plot</t>
-  </si>
-  <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Send SMS</t>
-  </si>
-  <si>
-    <t>DateTime Picker</t>
-  </si>
-  <si>
-    <t>Screen Female Client</t>
-  </si>
-  <si>
-    <t>Client 6 Week</t>
-  </si>
-  <si>
-    <t>Client 6 Month</t>
-  </si>
-  <si>
-    <t>Screen Partner</t>
-  </si>
-  <si>
-    <t>Partner 6 Month</t>
   </si>
   <si>
     <t>सामान्य जावास्क्रिप्ट फ़्रेमवर्क</t>
@@ -987,6 +783,75 @@
   </si>
   <si>
     <t>Medical Consultation</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('odontology')</t>
+  </si>
+  <si>
+    <t>odontology</t>
+  </si>
+  <si>
+    <t>Odontology</t>
+  </si>
+  <si>
+    <t>psychological</t>
+  </si>
+  <si>
+    <t>Psychological</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('psychological')</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('supply')</t>
+  </si>
+  <si>
+    <t>Medicine Supply</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('lab')</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>triage</t>
+  </si>
+  <si>
+    <t>Triage</t>
+  </si>
+  <si>
+    <t>add_test</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('add_test')</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('pickup')</t>
+  </si>
+  <si>
+    <t>Add Test</t>
+  </si>
+  <si>
+    <t>pickup</t>
+  </si>
+  <si>
+    <t>Pickup</t>
+  </si>
+  <si>
+    <t>update_supplies</t>
+  </si>
+  <si>
+    <t>Update Supplies</t>
+  </si>
+  <si>
+    <t>'?' +  odkSurvey.getHashString('update_supplies')</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1046,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1191,14 +1056,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1718,798 +1579,364 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" style="4"/>
-    <col min="2" max="2" width="101.1796875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="17.1796875" style="4"/>
+    <col min="1" max="1" width="17.1796875" style="3"/>
+    <col min="2" max="2" width="101.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="17.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="17.5" customHeight="1">
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" ht="41.25" customHeight="1">
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="5"/>
+      <c r="A8" s="7" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" s="5"/>
+      <c r="A11" s="7" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="5"/>
+      <c r="A14" s="7" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="59.25" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="59.25" customHeight="1">
+      <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" s="4" t="s">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4" t="s">
+    <row r="21" spans="1:7" ht="66" customHeight="1">
+      <c r="C21" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="4" t="s">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4" t="s">
+    <row r="24" spans="1:7" ht="66" customHeight="1">
+      <c r="C24" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="4" t="s">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A26" s="4"/>
+      <c r="B26" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4" t="s">
+    <row r="27" spans="1:7" ht="66" customHeight="1">
+      <c r="C27" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E27" s="4" t="s">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4" t="s">
+    <row r="30" spans="1:7" ht="66" customHeight="1">
+      <c r="C30" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E30" s="4" t="s">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A32" s="4"/>
+      <c r="B32" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="4" t="s">
+    <row r="33" spans="1:7" ht="66" customHeight="1">
+      <c r="C33" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="4" t="s">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A35" s="4"/>
+      <c r="B35" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4" t="s">
+    <row r="36" spans="1:7" ht="66" customHeight="1">
+      <c r="C36" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A38" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A47" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A53" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A56" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A59" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A62" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1">
-      <c r="A63" s="5"/>
-      <c r="B63" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A65" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1">
-      <c r="A66" s="5"/>
-      <c r="B66" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A68" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1">
-      <c r="A69" s="5"/>
-      <c r="B69" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A71" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17" customHeight="1">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A74" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="62" customHeight="1">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A77" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="62" customHeight="1">
-      <c r="A78" s="5"/>
-      <c r="B78" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="12" customHeight="1">
-      <c r="A80" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="58" customHeight="1">
-      <c r="A81" s="5"/>
-      <c r="B81" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="12" customHeight="1">
-      <c r="A83" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="58" customHeight="1">
-      <c r="A84" s="5"/>
-      <c r="B84" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="12" customHeight="1">
-      <c r="A86" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="58" customHeight="1">
-      <c r="A87" s="5"/>
-      <c r="B87" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A89" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="58" customHeight="1">
-      <c r="A90" s="5"/>
-      <c r="B90" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A91" s="5"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="12.5" customHeight="1">
-      <c r="A92" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="58.5" customHeight="1">
-      <c r="A93" s="5"/>
-      <c r="B93" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="12.75" customHeight="1">
-      <c r="C94" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="37" spans="1:7" ht="17.25" customHeight="1"/>
+    <row r="38" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="39" spans="1:7" ht="66" customHeight="1"/>
+    <row r="40" spans="1:7" ht="17.25" customHeight="1"/>
+    <row r="41" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="42" spans="1:7" ht="66" customHeight="1"/>
+    <row r="43" spans="1:7" ht="17.25" customHeight="1"/>
+    <row r="44" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="45" spans="1:7" ht="66" customHeight="1"/>
+    <row r="46" spans="1:7" ht="17.25" customHeight="1"/>
+    <row r="47" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="48" spans="1:7" ht="66" customHeight="1"/>
+    <row r="49" ht="17.25" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
+    <row r="51" ht="66" customHeight="1"/>
+    <row r="52" ht="17.25" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
+    <row r="54" ht="66" customHeight="1"/>
+    <row r="55" ht="17.25" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
+    <row r="57" ht="66" customHeight="1"/>
+    <row r="58" ht="17.25" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
+    <row r="60" ht="66" customHeight="1"/>
+    <row r="61" ht="17.25" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
+    <row r="63" ht="66" customHeight="1"/>
+    <row r="64" ht="17.25" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
+    <row r="66" ht="66" customHeight="1"/>
+    <row r="67" ht="17.25" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
+    <row r="69" ht="66" customHeight="1"/>
+    <row r="70" ht="17.25" customHeight="1"/>
+    <row r="71" ht="17.5" customHeight="1"/>
+    <row r="72" ht="66" customHeight="1"/>
+    <row r="73" ht="17" customHeight="1"/>
+    <row r="75" ht="62" customHeight="1"/>
+    <row r="78" ht="62" customHeight="1"/>
+    <row r="80" ht="12" customHeight="1"/>
+    <row r="81" ht="58" customHeight="1"/>
+    <row r="83" ht="12" customHeight="1"/>
+    <row r="84" ht="58" customHeight="1"/>
+    <row r="86" ht="12" customHeight="1"/>
+    <row r="87" ht="58" customHeight="1"/>
+    <row r="90" ht="58" customHeight="1"/>
+    <row r="92" ht="12.5" customHeight="1"/>
+    <row r="93" ht="58.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2544,22 +1971,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>294</v>
+        <v>226</v>
       </c>
       <c r="D1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="F1" t="s">
-        <v>295</v>
+        <v>227</v>
       </c>
       <c r="G1" t="s">
-        <v>299</v>
+        <v>231</v>
       </c>
       <c r="H1" t="s">
-        <v>231</v>
+        <v>163</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -2614,14 +2041,14 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>289</v>
+        <v>156</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
@@ -2633,44 +2060,44 @@
     <row r="6" spans="1:10" ht="18.75" customHeight="1"/>
     <row r="7" spans="1:10" ht="18.75" customHeight="1">
       <c r="A7" t="s">
-        <v>296</v>
+        <v>228</v>
       </c>
       <c r="F7" t="s">
         <v>154</v>
       </c>
       <c r="G7" t="s">
-        <v>302</v>
+        <v>234</v>
       </c>
       <c r="H7" t="s">
-        <v>232</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1">
       <c r="A8" t="s">
-        <v>297</v>
+        <v>229</v>
       </c>
       <c r="F8" t="s">
-        <v>209</v>
+        <v>155</v>
       </c>
       <c r="G8" t="s">
-        <v>300</v>
+        <v>232</v>
       </c>
       <c r="H8" t="s">
-        <v>209</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1">
       <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" t="s">
         <v>233</v>
       </c>
-      <c r="F9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G9" t="s">
-        <v>301</v>
-      </c>
       <c r="H9" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -2755,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -2780,322 +2207,113 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="B9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>183</v>
-      </c>
-      <c r="C16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>189</v>
-      </c>
-      <c r="C18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C20" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>199</v>
-      </c>
-      <c r="C24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>205</v>
-      </c>
-      <c r="C27" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>309</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3120,678 +2338,678 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.81640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.1796875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="4"/>
+    <col min="1" max="1" width="26.36328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="57.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="56.1796875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>230</v>
+      <c r="C1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>237</v>
+      <c r="D2" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>238</v>
+      <c r="D3" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>239</v>
+      <c r="D4" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>240</v>
+      <c r="D5" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>241</v>
+      <c r="D6" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>242</v>
+      <c r="C7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>243</v>
+      <c r="C8" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>244</v>
+      <c r="C9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>245</v>
+      <c r="C10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.75" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>246</v>
+      <c r="D11" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.75" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>239</v>
+      <c r="D12" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>247</v>
+      <c r="D13" s="3" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>248</v>
+      <c r="D14" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>249</v>
+      <c r="D15" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>250</v>
+      <c r="D16" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>251</v>
+      <c r="D17" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>252</v>
+      <c r="D18" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>253</v>
+      <c r="D19" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>254</v>
+      <c r="D20" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>255</v>
+      <c r="D21" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>256</v>
+      <c r="D22" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>257</v>
+      <c r="D23" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>258</v>
+      <c r="D24" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>259</v>
+      <c r="D26" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>260</v>
+      <c r="D27" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>261</v>
+      <c r="D28" s="7" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>290</v>
+      <c r="D29" s="7" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>262</v>
+      <c r="D30" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>263</v>
+      <c r="D31" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>264</v>
+      <c r="D33" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>265</v>
+      <c r="D34" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>266</v>
+      <c r="D35" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="175">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>291</v>
+      <c r="D36" s="7" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>267</v>
+      <c r="D37" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>268</v>
+      <c r="D38" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>269</v>
+      <c r="D39" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>270</v>
+      <c r="D40" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>271</v>
+      <c r="D41" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>272</v>
+      <c r="D42" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>273</v>
+      <c r="D43" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>274</v>
+      <c r="D44" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>275</v>
+      <c r="C45" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>276</v>
+      <c r="D46" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>277</v>
+      <c r="D47" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>278</v>
+      <c r="D48" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>279</v>
+      <c r="D49" s="7" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13" customHeight="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>280</v>
+      <c r="D50" s="7" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>281</v>
+      <c r="D51" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>263</v>
+      <c r="D52" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>282</v>
+      <c r="D53" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>277</v>
+      <c r="D54" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>283</v>
+      <c r="D55" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>284</v>
+      <c r="D56" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>285</v>
+      <c r="D57" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>286</v>
+      <c r="D58" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>287</v>
+      <c r="D59" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>288</v>
+      <c r="D60" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3828,13 +3046,13 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>292</v>
+        <v>224</v>
       </c>
       <c r="C1" t="s">
-        <v>293</v>
+        <v>225</v>
       </c>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>

</xml_diff>